<commit_message>
remove app notes, moved to drive
</commit_message>
<xml_diff>
--- a/Capstone Gantt Chart.xlsx
+++ b/Capstone Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\AndroidStudioProjects\AdditionalDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF0C9B0-85C8-49A6-A03B-DFBB7475F6D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A08A2-2096-46D5-A50E-317BDB394862}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>Final Report</t>
   </si>
   <si>
-    <t>Video</t>
-  </si>
-  <si>
     <t>Define UI</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>I/O Demo</t>
+  </si>
+  <si>
+    <t>Video + Final Presentation</t>
   </si>
 </sst>
 </file>
@@ -729,21 +729,6 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,6 +740,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,8 +1074,8 @@
   </sheetPr>
   <dimension ref="A1:BK996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1088,16 +1088,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1155,14 +1155,14 @@
       <c r="BK1" s="2"/>
     </row>
     <row r="2" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1220,14 +1220,14 @@
       <c r="BK2" s="2"/>
     </row>
     <row r="3" spans="1:63" ht="30" customHeight="1">
-      <c r="A3" s="95"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1285,115 +1285,115 @@
       <c r="BK3" s="7"/>
     </row>
     <row r="4" spans="1:63" ht="14.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="89" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="89" t="s">
+      <c r="E4" s="92" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="92" t="s">
+      <c r="H4" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="91" t="s">
+      <c r="I4" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="87" t="s">
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="87" t="s">
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="95"/>
+      <c r="X4" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88"/>
-      <c r="X4" s="87" t="s">
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="87" t="s">
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="AD4" s="88"/>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="87" t="s">
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="88"/>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="87" t="s">
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="87" t="s">
+      <c r="AS4" s="95"/>
+      <c r="AT4" s="95"/>
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="87" t="s">
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="95"/>
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="88"/>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="87" t="s">
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="95"/>
+      <c r="BG4" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="88"/>
-      <c r="BG4" s="87" t="s">
-        <v>48</v>
-      </c>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
+      <c r="BH4" s="95"/>
+      <c r="BI4" s="95"/>
+      <c r="BJ4" s="95"/>
+      <c r="BK4" s="95"/>
     </row>
     <row r="5" spans="1:63" ht="14.25">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="93"/>
+      <c r="A5" s="93"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="98"/>
       <c r="I5" s="35" t="s">
         <v>6</v>
       </c>
@@ -1565,12 +1565,12 @@
         <v>14</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="7" spans="1:63" ht="14.25">
       <c r="B7" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="16">
         <v>43494</v>
@@ -1727,7 +1727,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="18">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I8" s="19"/>
       <c r="J8" s="20"/>
@@ -1806,7 +1806,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="18">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I9" s="76"/>
       <c r="J9" s="77"/>
@@ -2043,7 +2043,7 @@
         <v>28</v>
       </c>
       <c r="H12" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="20"/>
@@ -2103,7 +2103,7 @@
     </row>
     <row r="13" spans="1:63" ht="14.25">
       <c r="B13" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="16">
         <v>43535</v>
@@ -2122,7 +2122,7 @@
         <v>28</v>
       </c>
       <c r="H13" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="19"/>
       <c r="J13" s="20"/>
@@ -2185,12 +2185,12 @@
         <v>15</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
       <c r="I14" s="26"/>
       <c r="J14" s="27"/>
       <c r="K14" s="28"/>
@@ -2265,7 +2265,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="29">
         <v>1</v>
@@ -2347,7 +2347,7 @@
         <v>27</v>
       </c>
       <c r="H16" s="29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I16" s="19"/>
       <c r="J16" s="20"/>
@@ -2426,7 +2426,7 @@
         <v>29</v>
       </c>
       <c r="H17" s="29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="20"/>
@@ -2502,10 +2502,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H18" s="29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I18" s="19"/>
       <c r="J18" s="20"/>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="19" spans="1:63" ht="14.25">
       <c r="B19" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="16">
         <v>43519</v>
@@ -2581,10 +2581,10 @@
         <v>21</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H19" s="29">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I19" s="19"/>
       <c r="J19" s="20"/>
@@ -2647,12 +2647,12 @@
         <v>16</v>
       </c>
       <c r="B20" s="25"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="28"/>
@@ -2727,10 +2727,10 @@
         <v>5</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H21" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I21" s="68"/>
       <c r="J21" s="69"/>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="22" spans="1:63" ht="14.25">
       <c r="B22" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="16">
         <v>43500</v>
@@ -2806,10 +2806,10 @@
         <v>10</v>
       </c>
       <c r="G22" s="86" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H22" s="30">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="I22" s="19"/>
       <c r="J22" s="20"/>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="23" spans="1:63" ht="14.25">
       <c r="B23" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="16">
         <v>43512</v>
@@ -2888,7 +2888,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="30">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I23" s="19"/>
       <c r="J23" s="20"/>
@@ -2948,7 +2948,7 @@
     </row>
     <row r="24" spans="1:63" ht="14.25">
       <c r="B24" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="16">
         <v>43512</v>
@@ -2967,7 +2967,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="30">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I24" s="19"/>
       <c r="J24" s="20"/>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="25" spans="1:63" ht="14.25">
       <c r="B25" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="16">
         <v>43519</v>
@@ -3046,7 +3046,7 @@
         <v>11</v>
       </c>
       <c r="H25" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="19"/>
       <c r="J25" s="20"/>
@@ -3109,12 +3109,12 @@
         <v>17</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="96"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="28"/>
@@ -3268,7 +3268,7 @@
         <v>8</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H28" s="30">
         <v>1</v>
@@ -3331,7 +3331,7 @@
     </row>
     <row r="29" spans="1:63" ht="14.25">
       <c r="B29" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="16">
         <v>43509</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="30" spans="1:63" ht="14.25">
       <c r="B30" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="16">
         <v>43549</v>
@@ -3426,7 +3426,7 @@
         <v>10</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H30" s="30">
         <v>1</v>
@@ -3508,7 +3508,7 @@
         <v>27</v>
       </c>
       <c r="H31" s="30">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="20"/>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="32" spans="1:63" ht="14.25">
       <c r="B32" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="16">
         <v>43529</v>
@@ -3587,7 +3587,7 @@
         <v>27</v>
       </c>
       <c r="H32" s="30">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="20"/>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="33" spans="1:63" ht="14.25">
       <c r="B33" s="15" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C33" s="16">
         <v>43529</v>
@@ -3663,7 +3663,7 @@
         <v>27</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H33" s="30">
         <v>0</v>
@@ -6684,16 +6684,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="AM4:AQ4"/>
     <mergeCell ref="AH4:AL4"/>
     <mergeCell ref="C4:C5"/>
@@ -6708,6 +6698,16 @@
     <mergeCell ref="BB4:BF4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:H19">
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
Updated gant chart for capstone
</commit_message>
<xml_diff>
--- a/Capstone Gantt Chart.xlsx
+++ b/Capstone Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\AndroidStudioProjects\AdditionalDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172A08A2-2096-46D5-A50E-317BDB394862}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC698DD7-67CF-4F74-9737-9C98C5FCCECD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,6 +729,21 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,21 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1074,8 +1074,8 @@
   </sheetPr>
   <dimension ref="A1:BK996"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1088,16 +1088,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1155,14 +1155,14 @@
       <c r="BK1" s="2"/>
     </row>
     <row r="2" spans="1:63" ht="15.75" customHeight="1">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1220,14 +1220,14 @@
       <c r="BK2" s="2"/>
     </row>
     <row r="3" spans="1:63" ht="30" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1285,115 +1285,115 @@
       <c r="BK3" s="7"/>
     </row>
     <row r="4" spans="1:63" ht="14.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92" t="s">
+      <c r="A4" s="89"/>
+      <c r="B4" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="92" t="s">
+      <c r="G4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="96" t="s">
+      <c r="I4" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="94" t="s">
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="94" t="s">
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="95"/>
-      <c r="U4" s="95"/>
-      <c r="V4" s="95"/>
-      <c r="W4" s="95"/>
-      <c r="X4" s="94" t="s">
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="95"/>
-      <c r="AB4" s="95"/>
-      <c r="AC4" s="94" t="s">
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="95"/>
-      <c r="AH4" s="94" t="s">
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="AI4" s="95"/>
-      <c r="AJ4" s="95"/>
-      <c r="AK4" s="95"/>
-      <c r="AL4" s="95"/>
-      <c r="AM4" s="94" t="s">
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="88"/>
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="AN4" s="95"/>
-      <c r="AO4" s="95"/>
-      <c r="AP4" s="95"/>
-      <c r="AQ4" s="95"/>
-      <c r="AR4" s="94" t="s">
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="AS4" s="95"/>
-      <c r="AT4" s="95"/>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="94" t="s">
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AX4" s="95"/>
-      <c r="AY4" s="95"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="95"/>
-      <c r="BB4" s="94" t="s">
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="88"/>
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="95"/>
-      <c r="BF4" s="95"/>
-      <c r="BG4" s="94" t="s">
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="88"/>
+      <c r="BG4" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="BH4" s="95"/>
-      <c r="BI4" s="95"/>
-      <c r="BJ4" s="95"/>
-      <c r="BK4" s="95"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
     </row>
     <row r="5" spans="1:63" ht="14.25">
-      <c r="A5" s="93"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
-      <c r="H5" s="98"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="93"/>
       <c r="I5" s="35" t="s">
         <v>6</v>
       </c>
@@ -1565,12 +1565,12 @@
         <v>14</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="14"/>
@@ -2185,12 +2185,12 @@
         <v>15</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
       <c r="I14" s="26"/>
       <c r="J14" s="27"/>
       <c r="K14" s="28"/>
@@ -2647,12 +2647,12 @@
         <v>16</v>
       </c>
       <c r="B20" s="25"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="28"/>
@@ -3109,12 +3109,12 @@
         <v>17</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="90"/>
-      <c r="E26" s="90"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="28"/>
@@ -3508,7 +3508,7 @@
         <v>27</v>
       </c>
       <c r="H31" s="30">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="20"/>
@@ -3587,7 +3587,7 @@
         <v>27</v>
       </c>
       <c r="H32" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I32" s="19"/>
       <c r="J32" s="20"/>
@@ -3666,7 +3666,7 @@
         <v>49</v>
       </c>
       <c r="H33" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="19"/>
       <c r="J33" s="20"/>
@@ -6684,6 +6684,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="AM4:AQ4"/>
     <mergeCell ref="AH4:AL4"/>
     <mergeCell ref="C4:C5"/>
@@ -6698,16 +6708,6 @@
     <mergeCell ref="BB4:BF4"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="H17:H19">
     <cfRule type="colorScale" priority="5">

</xml_diff>